<commit_message>
[A1#111#SAXOSXX/Saxos_Informatica_S.R.L./ProgettoOsp/11.108]: Fix report-checklist file
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#SAXOSXX/Saxos_Informatica_S.R.L./ProgettoOsp/11.108/report-checklist.xlsx
+++ b/GATEWAY/A1#111#SAXOSXX/Saxos_Informatica_S.R.L./ProgettoOsp/11.108/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Simone\Documents\GitHub\it-fse-accreditamento-main\GATEWAY\A1#111#SAXOSXX\Saxos_Informatica_S.R.L\ProgettoOsp\11.108\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Simone\Documents\HL7\FSE2.0\Gateway Sogei\Accreditamento Validazione RSA-RAD-LDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF71B1BA-A959-4FE8-B8EF-0F07FFE08337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA93C831-D242-4F18-A4FA-54C28E394A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="904">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -5117,6 +5117,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5138,15 +5147,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7612,10 +7612,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A66" sqref="A66"/>
+      <selection pane="bottomRight" activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7660,14 +7660,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="40" t="s">
         <v>851</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="39"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7685,14 +7685,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="47" t="s">
         <v>849</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="39"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7710,12 +7710,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="47" t="s">
         <v>848</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7734,12 +7734,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
         <v>850</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="39"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7757,8 +7757,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -9806,7 +9806,7 @@
       <c r="J66" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K66" s="45" t="s">
+      <c r="K66" s="33" t="s">
         <v>852</v>
       </c>
       <c r="L66" s="25"/>
@@ -9844,7 +9844,7 @@
       <c r="J67" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K67" s="45" t="s">
+      <c r="K67" s="33" t="s">
         <v>853</v>
       </c>
       <c r="L67" s="25"/>
@@ -9889,11 +9889,11 @@
       <c r="M68" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="N68" s="45"/>
+      <c r="N68" s="33"/>
       <c r="O68" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="P68" s="45" t="s">
+      <c r="P68" s="33" t="s">
         <v>854</v>
       </c>
       <c r="Q68" s="25"/>
@@ -9915,7 +9915,7 @@
       <c r="C69" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="D69" s="46" t="s">
+      <c r="D69" s="34" t="s">
         <v>336</v>
       </c>
       <c r="E69" s="22" t="s">
@@ -9928,7 +9928,7 @@
       <c r="J69" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K69" s="45" t="s">
+      <c r="K69" s="33" t="s">
         <v>899</v>
       </c>
       <c r="L69" s="25"/>
@@ -9966,7 +9966,7 @@
       <c r="J70" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K70" s="45" t="s">
+      <c r="K70" s="33" t="s">
         <v>858</v>
       </c>
       <c r="L70" s="25"/>
@@ -10004,7 +10004,7 @@
       <c r="J71" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K71" s="45" t="s">
+      <c r="K71" s="33" t="s">
         <v>858</v>
       </c>
       <c r="L71" s="25"/>
@@ -10042,7 +10042,7 @@
       <c r="J72" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K72" s="45" t="s">
+      <c r="K72" s="33" t="s">
         <v>858</v>
       </c>
       <c r="L72" s="25"/>
@@ -10067,7 +10067,7 @@
       <c r="C73" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="D73" s="46" t="s">
+      <c r="D73" s="34" t="s">
         <v>344</v>
       </c>
       <c r="E73" s="22" t="s">
@@ -10080,7 +10080,7 @@
       <c r="J73" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K73" s="45" t="s">
+      <c r="K73" s="33" t="s">
         <v>859</v>
       </c>
       <c r="L73" s="25"/>
@@ -10118,7 +10118,7 @@
       <c r="J74" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K74" s="45" t="s">
+      <c r="K74" s="33" t="s">
         <v>860</v>
       </c>
       <c r="L74" s="25"/>
@@ -10156,7 +10156,7 @@
       <c r="J75" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K75" s="45" t="s">
+      <c r="K75" s="33" t="s">
         <v>861</v>
       </c>
       <c r="L75" s="25"/>
@@ -10194,7 +10194,7 @@
       <c r="J76" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K76" s="45" t="s">
+      <c r="K76" s="33" t="s">
         <v>862</v>
       </c>
       <c r="L76" s="25"/>
@@ -10232,7 +10232,7 @@
       <c r="J77" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K77" s="45" t="s">
+      <c r="K77" s="33" t="s">
         <v>863</v>
       </c>
       <c r="L77" s="25"/>
@@ -10270,7 +10270,7 @@
       <c r="J78" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K78" s="45" t="s">
+      <c r="K78" s="33" t="s">
         <v>865</v>
       </c>
       <c r="L78" s="25"/>
@@ -10308,7 +10308,7 @@
       <c r="J79" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K79" s="45" t="s">
+      <c r="K79" s="33" t="s">
         <v>864</v>
       </c>
       <c r="L79" s="25"/>
@@ -10346,7 +10346,7 @@
       <c r="J80" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K80" s="45" t="s">
+      <c r="K80" s="33" t="s">
         <v>866</v>
       </c>
       <c r="L80" s="25"/>
@@ -10384,7 +10384,7 @@
       <c r="J81" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K81" s="45" t="s">
+      <c r="K81" s="33" t="s">
         <v>867</v>
       </c>
       <c r="L81" s="25"/>
@@ -10422,7 +10422,7 @@
       <c r="J82" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K82" s="45" t="s">
+      <c r="K82" s="33" t="s">
         <v>868</v>
       </c>
       <c r="L82" s="25"/>
@@ -10460,7 +10460,7 @@
       <c r="J83" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K83" s="45" t="s">
+      <c r="K83" s="33" t="s">
         <v>869</v>
       </c>
       <c r="L83" s="25"/>
@@ -10498,7 +10498,7 @@
       <c r="J84" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K84" s="45" t="s">
+      <c r="K84" s="33" t="s">
         <v>870</v>
       </c>
       <c r="L84" s="25"/>
@@ -10536,7 +10536,7 @@
       <c r="J85" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K85" s="45" t="s">
+      <c r="K85" s="33" t="s">
         <v>871</v>
       </c>
       <c r="L85" s="25"/>
@@ -10574,7 +10574,7 @@
       <c r="J86" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K86" s="45" t="s">
+      <c r="K86" s="33" t="s">
         <v>872</v>
       </c>
       <c r="L86" s="25"/>
@@ -10612,7 +10612,7 @@
       <c r="J87" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K87" s="45" t="s">
+      <c r="K87" s="33" t="s">
         <v>872</v>
       </c>
       <c r="L87" s="25"/>
@@ -10650,7 +10650,7 @@
       <c r="J88" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K88" s="45" t="s">
+      <c r="K88" s="33" t="s">
         <v>872</v>
       </c>
       <c r="L88" s="25"/>
@@ -10688,7 +10688,7 @@
       <c r="J89" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K89" s="45" t="s">
+      <c r="K89" s="33" t="s">
         <v>872</v>
       </c>
       <c r="L89" s="25"/>
@@ -10741,11 +10741,11 @@
       <c r="M90" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="N90" s="45"/>
+      <c r="N90" s="33"/>
       <c r="O90" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P90" s="45" t="s">
+      <c r="P90" s="33" t="s">
         <v>876</v>
       </c>
       <c r="Q90" s="25"/>
@@ -10778,7 +10778,7 @@
       <c r="J91" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K91" s="45" t="s">
+      <c r="K91" s="33" t="s">
         <v>877</v>
       </c>
       <c r="L91" s="25"/>
@@ -10812,13 +10812,13 @@
       <c r="F92" s="23">
         <v>45376</v>
       </c>
-      <c r="G92" s="47" t="s">
+      <c r="G92" s="35" t="s">
         <v>855</v>
       </c>
-      <c r="H92" s="47" t="s">
+      <c r="H92" s="35" t="s">
         <v>856</v>
       </c>
-      <c r="I92" s="47" t="s">
+      <c r="I92" s="35" t="s">
         <v>857</v>
       </c>
       <c r="J92" s="25" t="s">
@@ -10859,10 +10859,10 @@
       <c r="G93" s="24" t="s">
         <v>888</v>
       </c>
-      <c r="H93" s="47" t="s">
+      <c r="H93" s="35" t="s">
         <v>889</v>
       </c>
-      <c r="I93" s="47" t="s">
+      <c r="I93" s="35" t="s">
         <v>890</v>
       </c>
       <c r="J93" s="25" t="s">
@@ -10904,7 +10904,7 @@
       <c r="J94" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K94" s="45" t="s">
+      <c r="K94" s="33" t="s">
         <v>881</v>
       </c>
       <c r="L94" s="25"/>
@@ -10942,7 +10942,7 @@
       <c r="J95" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K95" s="45" t="s">
+      <c r="K95" s="33" t="s">
         <v>858</v>
       </c>
       <c r="L95" s="25"/>
@@ -10980,7 +10980,7 @@
       <c r="J96" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K96" s="45" t="s">
+      <c r="K96" s="33" t="s">
         <v>858</v>
       </c>
       <c r="L96" s="25"/>
@@ -11018,7 +11018,7 @@
       <c r="J97" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K97" s="45" t="s">
+      <c r="K97" s="33" t="s">
         <v>852</v>
       </c>
       <c r="L97" s="25"/>
@@ -11056,7 +11056,7 @@
       <c r="J98" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K98" s="45" t="s">
+      <c r="K98" s="33" t="s">
         <v>853</v>
       </c>
       <c r="L98" s="25"/>
@@ -11105,7 +11105,7 @@
       <c r="O99" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="P99" s="45" t="s">
+      <c r="P99" s="33" t="s">
         <v>854</v>
       </c>
       <c r="Q99" s="25"/>
@@ -11140,7 +11140,7 @@
       <c r="J100" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K100" s="45" t="s">
+      <c r="K100" s="33" t="s">
         <v>859</v>
       </c>
       <c r="L100" s="25"/>
@@ -11178,7 +11178,7 @@
       <c r="J101" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K101" s="45" t="s">
+      <c r="K101" s="33" t="s">
         <v>860</v>
       </c>
       <c r="L101" s="25"/>
@@ -11368,7 +11368,7 @@
       <c r="J106" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K106" s="45" t="s">
+      <c r="K106" s="33" t="s">
         <v>882</v>
       </c>
       <c r="L106" s="25"/>
@@ -11558,7 +11558,7 @@
       <c r="J111" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K111" s="45" t="s">
+      <c r="K111" s="33" t="s">
         <v>883</v>
       </c>
       <c r="L111" s="25"/>
@@ -11596,7 +11596,7 @@
       <c r="J112" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K112" s="45" t="s">
+      <c r="K112" s="33" t="s">
         <v>884</v>
       </c>
       <c r="L112" s="25"/>
@@ -11795,11 +11795,19 @@
         <v>138</v>
       </c>
       <c r="K117" s="25"/>
-      <c r="L117" s="25"/>
-      <c r="M117" s="25"/>
+      <c r="L117" s="25" t="s">
+        <v>847</v>
+      </c>
+      <c r="M117" s="25" t="s">
+        <v>847</v>
+      </c>
       <c r="N117" s="25"/>
-      <c r="O117" s="25"/>
-      <c r="P117" s="25"/>
+      <c r="O117" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="P117" s="33" t="s">
+        <v>876</v>
+      </c>
       <c r="Q117" s="25"/>
       <c r="R117" s="26"/>
       <c r="S117" s="27"/>
@@ -11830,7 +11838,7 @@
       <c r="J118" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K118" s="45" t="s">
+      <c r="K118" s="33" t="s">
         <v>891</v>
       </c>
       <c r="L118" s="25"/>
@@ -11909,8 +11917,8 @@
       <c r="G120" s="24"/>
       <c r="H120" s="24"/>
       <c r="I120" s="24"/>
-      <c r="J120" s="45"/>
-      <c r="K120" s="45"/>
+      <c r="J120" s="33"/>
+      <c r="K120" s="33"/>
       <c r="L120" s="25"/>
       <c r="M120" s="25"/>
       <c r="N120" s="25"/>
@@ -12764,7 +12772,7 @@
       <c r="J145" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K145" s="45" t="s">
+      <c r="K145" s="33" t="s">
         <v>895</v>
       </c>
       <c r="L145" s="25"/>
@@ -12916,7 +12924,7 @@
       <c r="J149" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K149" s="45" t="s">
+      <c r="K149" s="33" t="s">
         <v>852</v>
       </c>
       <c r="L149" s="25"/>
@@ -12954,7 +12962,7 @@
       <c r="J150" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K150" s="45" t="s">
+      <c r="K150" s="33" t="s">
         <v>853</v>
       </c>
       <c r="L150" s="25"/>
@@ -13003,7 +13011,7 @@
       <c r="O151" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="P151" s="45" t="s">
+      <c r="P151" s="33" t="s">
         <v>854</v>
       </c>
       <c r="Q151" s="25"/>
@@ -13266,7 +13274,7 @@
       <c r="J158" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K158" s="45" t="s">
+      <c r="K158" s="33" t="s">
         <v>896</v>
       </c>
       <c r="L158" s="25"/>
@@ -13304,7 +13312,7 @@
       <c r="J159" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K159" s="45" t="s">
+      <c r="K159" s="33" t="s">
         <v>897</v>
       </c>
       <c r="L159" s="25"/>
@@ -13342,7 +13350,7 @@
       <c r="J160" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K160" s="45" t="s">
+      <c r="K160" s="33" t="s">
         <v>898</v>
       </c>
       <c r="L160" s="25"/>
@@ -13380,7 +13388,7 @@
       <c r="J161" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K161" s="45" t="s">
+      <c r="K161" s="33" t="s">
         <v>900</v>
       </c>
       <c r="L161" s="25"/>
@@ -13470,7 +13478,7 @@
       <c r="J163" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K163" s="45" t="s">
+      <c r="K163" s="33" t="s">
         <v>900</v>
       </c>
       <c r="L163" s="25"/>
@@ -13513,7 +13521,7 @@
       <c r="I164" s="24" t="s">
         <v>894</v>
       </c>
-      <c r="J164" s="45" t="s">
+      <c r="J164" s="33" t="s">
         <v>138</v>
       </c>
       <c r="K164" s="25"/>
@@ -13529,7 +13537,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="20">
         <v>1</v>
       </c>
@@ -13563,7 +13571,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="20">
         <v>2</v>
       </c>
@@ -13597,7 +13605,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="20">
         <v>3</v>
       </c>
@@ -13631,7 +13639,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="20">
         <v>4</v>
       </c>
@@ -13665,7 +13673,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="20">
         <v>5</v>
       </c>
@@ -13699,7 +13707,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="20">
         <v>28</v>
       </c>
@@ -13733,7 +13741,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="20">
         <v>36</v>
       </c>
@@ -13767,7 +13775,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="20">
         <v>44</v>
       </c>
@@ -13803,7 +13811,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="20">
         <v>52</v>
       </c>
@@ -13837,7 +13845,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="20">
         <v>53</v>
       </c>
@@ -13871,7 +13879,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="20">
         <v>54</v>
       </c>
@@ -13905,7 +13913,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="20">
         <v>55</v>
       </c>
@@ -13939,7 +13947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="20">
         <v>56</v>
       </c>
@@ -13973,7 +13981,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="20">
         <v>57</v>
       </c>
@@ -14007,7 +14015,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="20">
         <v>58</v>
       </c>
@@ -14041,7 +14049,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="20">
         <v>59</v>
       </c>
@@ -14075,7 +14083,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="20">
         <v>60</v>
       </c>
@@ -14109,7 +14117,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="20">
         <v>61</v>
       </c>
@@ -14143,7 +14151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="20">
         <v>62</v>
       </c>
@@ -14177,7 +14185,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="20">
         <v>191</v>
       </c>
@@ -14211,7 +14219,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="20">
         <v>368</v>
       </c>
@@ -14245,7 +14253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="20">
         <v>376</v>
       </c>
@@ -14279,7 +14287,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="20">
         <v>16</v>
       </c>
@@ -14313,7 +14321,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="20">
         <v>17</v>
       </c>
@@ -14347,7 +14355,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="20">
         <v>18</v>
       </c>
@@ -14381,7 +14389,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="20">
         <v>19</v>
       </c>
@@ -14415,7 +14423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="20">
         <v>33</v>
       </c>
@@ -14449,7 +14457,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="20">
         <v>41</v>
       </c>
@@ -14483,7 +14491,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="20">
         <v>49</v>
       </c>
@@ -14519,7 +14527,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="20">
         <v>94</v>
       </c>
@@ -14553,7 +14561,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="20">
         <v>95</v>
       </c>
@@ -14587,7 +14595,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="20">
         <v>96</v>
       </c>
@@ -14621,7 +14629,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="20">
         <v>97</v>
       </c>
@@ -14655,7 +14663,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="20">
         <v>98</v>
       </c>
@@ -14689,7 +14697,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="241.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" ht="241.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="20">
         <v>99</v>
       </c>
@@ -14723,7 +14731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="301.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" ht="301.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="20">
         <v>100</v>
       </c>
@@ -14757,7 +14765,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="20">
         <v>101</v>
       </c>
@@ -14791,7 +14799,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="20">
         <v>102</v>
       </c>
@@ -14825,7 +14833,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="20">
         <v>103</v>
       </c>
@@ -14859,7 +14867,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="20">
         <v>104</v>
       </c>
@@ -14893,7 +14901,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="20">
         <v>105</v>
       </c>
@@ -14927,7 +14935,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="20">
         <v>106</v>
       </c>
@@ -14995,7 +15003,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="20">
         <v>193</v>
       </c>
@@ -15029,7 +15037,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="20">
         <v>206</v>
       </c>
@@ -15063,7 +15071,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="20">
         <v>209</v>
       </c>
@@ -15097,7 +15105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="20">
         <v>222</v>
       </c>
@@ -15131,7 +15139,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="20">
         <v>225</v>
       </c>
@@ -15165,7 +15173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="20">
         <v>238</v>
       </c>
@@ -15199,7 +15207,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="20">
         <v>241</v>
       </c>
@@ -15233,7 +15241,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="236.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" ht="236.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="20">
         <v>254</v>
       </c>
@@ -15267,7 +15275,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="20">
         <v>257</v>
       </c>
@@ -15301,7 +15309,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="284.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" ht="284.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="20">
         <v>270</v>
       </c>
@@ -15335,7 +15343,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="20">
         <v>273</v>
       </c>
@@ -15369,7 +15377,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="267.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" ht="267.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="20">
         <v>286</v>
       </c>
@@ -15403,7 +15411,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="20">
         <v>289</v>
       </c>
@@ -15437,7 +15445,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="20">
         <v>302</v>
       </c>
@@ -15471,7 +15479,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="20">
         <v>305</v>
       </c>
@@ -15505,7 +15513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="20">
         <v>318</v>
       </c>
@@ -15539,7 +15547,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="20">
         <v>322</v>
       </c>
@@ -15573,7 +15581,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="20">
         <v>323</v>
       </c>
@@ -15607,7 +15615,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="20">
         <v>326</v>
       </c>
@@ -15641,7 +15649,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="20">
         <v>327</v>
       </c>
@@ -15675,7 +15683,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="268.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:20" ht="268.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="20">
         <v>330</v>
       </c>
@@ -15709,7 +15717,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="20">
         <v>331</v>
       </c>
@@ -15743,7 +15751,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="20">
         <v>334</v>
       </c>
@@ -15777,7 +15785,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="204" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:20" ht="204" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="20">
         <v>335</v>
       </c>
@@ -15811,7 +15819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="20">
         <v>338</v>
       </c>
@@ -15845,7 +15853,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="20">
         <v>339</v>
       </c>
@@ -15879,7 +15887,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="20">
         <v>342</v>
       </c>
@@ -15913,7 +15921,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="20">
         <v>343</v>
       </c>
@@ -15947,7 +15955,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="20">
         <v>346</v>
       </c>
@@ -15981,7 +15989,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="20">
         <v>347</v>
       </c>
@@ -16015,7 +16023,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="20">
         <v>350</v>
       </c>
@@ -16049,7 +16057,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="20">
         <v>351</v>
       </c>
@@ -16083,7 +16091,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="20">
         <v>192</v>
       </c>
@@ -16117,7 +16125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="20">
         <v>197</v>
       </c>
@@ -16151,7 +16159,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="20">
         <v>198</v>
       </c>
@@ -16185,7 +16193,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="20">
         <v>199</v>
       </c>
@@ -16219,7 +16227,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="20">
         <v>200</v>
       </c>
@@ -16253,7 +16261,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="20">
         <v>201</v>
       </c>
@@ -16287,7 +16295,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="20">
         <v>202</v>
       </c>
@@ -16321,7 +16329,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="20">
         <v>203</v>
       </c>
@@ -16355,7 +16363,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="20">
         <v>208</v>
       </c>
@@ -16389,7 +16397,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="20">
         <v>213</v>
       </c>
@@ -16423,7 +16431,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="20">
         <v>214</v>
       </c>
@@ -16457,7 +16465,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="20">
         <v>215</v>
       </c>
@@ -16491,7 +16499,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="20">
         <v>216</v>
       </c>
@@ -16525,7 +16533,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="20">
         <v>217</v>
       </c>
@@ -16559,7 +16567,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="20">
         <v>218</v>
       </c>
@@ -16593,7 +16601,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="20">
         <v>219</v>
       </c>
@@ -16627,7 +16635,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="20">
         <v>224</v>
       </c>
@@ -16661,7 +16669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="20">
         <v>229</v>
       </c>
@@ -16695,7 +16703,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="20">
         <v>230</v>
       </c>
@@ -16729,7 +16737,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="20">
         <v>231</v>
       </c>
@@ -16763,7 +16771,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="20">
         <v>232</v>
       </c>
@@ -16797,7 +16805,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="20">
         <v>233</v>
       </c>
@@ -16831,7 +16839,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="20">
         <v>234</v>
       </c>
@@ -16865,7 +16873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="20">
         <v>235</v>
       </c>
@@ -16899,7 +16907,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="20">
         <v>240</v>
       </c>
@@ -16933,7 +16941,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="20">
         <v>245</v>
       </c>
@@ -16967,7 +16975,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="20">
         <v>246</v>
       </c>
@@ -17001,7 +17009,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="20">
         <v>247</v>
       </c>
@@ -17035,7 +17043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="20">
         <v>248</v>
       </c>
@@ -17069,7 +17077,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="20">
         <v>249</v>
       </c>
@@ -17103,7 +17111,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="20">
         <v>250</v>
       </c>
@@ -17137,7 +17145,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="20">
         <v>251</v>
       </c>
@@ -17171,7 +17179,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="20">
         <v>256</v>
       </c>
@@ -17205,7 +17213,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="20">
         <v>261</v>
       </c>
@@ -17239,7 +17247,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="20">
         <v>262</v>
       </c>
@@ -17273,7 +17281,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="20">
         <v>263</v>
       </c>
@@ -17307,7 +17315,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="20">
         <v>264</v>
       </c>
@@ -17341,7 +17349,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="20">
         <v>265</v>
       </c>
@@ -17375,7 +17383,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="20">
         <v>266</v>
       </c>
@@ -17409,7 +17417,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="237" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:20" ht="237" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="20">
         <v>267</v>
       </c>
@@ -17443,7 +17451,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="20">
         <v>272</v>
       </c>
@@ -17477,7 +17485,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="20">
         <v>277</v>
       </c>
@@ -17511,7 +17519,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="20">
         <v>278</v>
       </c>
@@ -17545,7 +17553,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="20">
         <v>279</v>
       </c>
@@ -17579,7 +17587,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="20">
         <v>280</v>
       </c>
@@ -17613,7 +17621,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="20">
         <v>281</v>
       </c>
@@ -17647,7 +17655,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="20">
         <v>282</v>
       </c>
@@ -17681,7 +17689,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="20">
         <v>283</v>
       </c>
@@ -17715,7 +17723,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="20">
         <v>288</v>
       </c>
@@ -17749,7 +17757,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="20">
         <v>293</v>
       </c>
@@ -17783,7 +17791,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="20">
         <v>294</v>
       </c>
@@ -17817,7 +17825,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="20">
         <v>295</v>
       </c>
@@ -17851,7 +17859,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="20">
         <v>296</v>
       </c>
@@ -17885,7 +17893,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="20">
         <v>297</v>
       </c>
@@ -17919,7 +17927,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="263.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:20" ht="263.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="20">
         <v>298</v>
       </c>
@@ -17953,7 +17961,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="264" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:20" ht="264" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="20">
         <v>299</v>
       </c>
@@ -17987,7 +17995,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="20">
         <v>304</v>
       </c>
@@ -18021,7 +18029,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="20">
         <v>309</v>
       </c>
@@ -18055,7 +18063,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="20">
         <v>310</v>
       </c>
@@ -18089,7 +18097,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="20">
         <v>311</v>
       </c>
@@ -18123,7 +18131,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="20">
         <v>312</v>
       </c>
@@ -18157,7 +18165,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="20">
         <v>313</v>
       </c>
@@ -18191,7 +18199,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="20">
         <v>314</v>
       </c>
@@ -18225,7 +18233,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="20">
         <v>315</v>
       </c>
@@ -18259,7 +18267,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="20">
         <v>320</v>
       </c>
@@ -18293,7 +18301,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="20">
         <v>321</v>
       </c>
@@ -18327,7 +18335,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="20">
         <v>324</v>
       </c>
@@ -18361,7 +18369,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="20">
         <v>325</v>
       </c>
@@ -18395,7 +18403,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="20">
         <v>328</v>
       </c>
@@ -18429,7 +18437,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="20">
         <v>329</v>
       </c>
@@ -18463,7 +18471,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="20">
         <v>332</v>
       </c>
@@ -18497,7 +18505,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="20">
         <v>333</v>
       </c>
@@ -18531,7 +18539,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="20">
         <v>336</v>
       </c>
@@ -18565,7 +18573,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="20">
         <v>337</v>
       </c>
@@ -18599,7 +18607,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="20">
         <v>340</v>
       </c>
@@ -18633,7 +18641,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="20">
         <v>341</v>
       </c>
@@ -18667,7 +18675,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="20">
         <v>344</v>
       </c>
@@ -18701,7 +18709,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="20">
         <v>345</v>
       </c>
@@ -18735,7 +18743,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="20">
         <v>348</v>
       </c>
@@ -18769,7 +18777,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="20">
         <v>349</v>
       </c>
@@ -18803,7 +18811,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="20">
         <v>196</v>
       </c>
@@ -18837,7 +18845,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="20">
         <v>207</v>
       </c>
@@ -18871,7 +18879,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="20">
         <v>212</v>
       </c>
@@ -18905,7 +18913,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="20">
         <v>223</v>
       </c>
@@ -18939,7 +18947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="253.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:20" ht="253.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="20">
         <v>228</v>
       </c>
@@ -18973,7 +18981,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="282.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:20" ht="282.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="20">
         <v>239</v>
       </c>
@@ -19007,7 +19015,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="20">
         <v>244</v>
       </c>
@@ -19041,7 +19049,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="20">
         <v>255</v>
       </c>
@@ -19075,7 +19083,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="20">
         <v>260</v>
       </c>
@@ -19109,7 +19117,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="20">
         <v>271</v>
       </c>
@@ -19143,7 +19151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="20">
         <v>276</v>
       </c>
@@ -19177,7 +19185,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="20">
         <v>287</v>
       </c>
@@ -19211,7 +19219,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" s="20">
         <v>292</v>
       </c>
@@ -19245,7 +19253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="20">
         <v>303</v>
       </c>
@@ -19279,7 +19287,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="20">
         <v>308</v>
       </c>
@@ -19313,7 +19321,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="20">
         <v>319</v>
       </c>
@@ -19347,7 +19355,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="20">
         <v>195</v>
       </c>
@@ -19381,7 +19389,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" s="20">
         <v>204</v>
       </c>
@@ -19415,7 +19423,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" s="20">
         <v>211</v>
       </c>
@@ -19449,7 +19457,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A339" s="20">
         <v>220</v>
       </c>
@@ -19483,7 +19491,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" s="20">
         <v>227</v>
       </c>
@@ -19517,7 +19525,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" s="20">
         <v>236</v>
       </c>
@@ -19551,7 +19559,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" s="20">
         <v>243</v>
       </c>
@@ -19585,7 +19593,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" s="20">
         <v>252</v>
       </c>
@@ -19619,7 +19627,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" s="20">
         <v>259</v>
       </c>
@@ -19653,7 +19661,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="20">
         <v>268</v>
       </c>
@@ -19687,7 +19695,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" s="20">
         <v>275</v>
       </c>
@@ -19721,7 +19729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" s="20">
         <v>284</v>
       </c>
@@ -19755,7 +19763,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" s="20">
         <v>291</v>
       </c>
@@ -19789,7 +19797,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" s="20">
         <v>300</v>
       </c>
@@ -19823,7 +19831,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" s="20">
         <v>307</v>
       </c>
@@ -19857,7 +19865,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" s="20">
         <v>316</v>
       </c>
@@ -19891,7 +19899,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="20">
         <v>194</v>
       </c>
@@ -19925,7 +19933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" s="20">
         <v>205</v>
       </c>
@@ -19959,7 +19967,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" s="20">
         <v>210</v>
       </c>
@@ -19993,7 +20001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" s="20">
         <v>221</v>
       </c>
@@ -20027,7 +20035,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356" s="20">
         <v>226</v>
       </c>
@@ -20061,7 +20069,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:20" ht="315" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357" s="20">
         <v>237</v>
       </c>
@@ -20095,7 +20103,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:20" ht="259.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A358" s="20">
         <v>242</v>
       </c>
@@ -20129,7 +20137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="20">
         <v>253</v>
       </c>
@@ -20163,7 +20171,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360" s="20">
         <v>258</v>
       </c>
@@ -20197,7 +20205,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361" s="20">
         <v>269</v>
       </c>
@@ -20231,7 +20239,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A362" s="20">
         <v>274</v>
       </c>
@@ -20265,7 +20273,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A363" s="20">
         <v>285</v>
       </c>
@@ -20299,7 +20307,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="20">
         <v>290</v>
       </c>
@@ -20333,7 +20341,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365" s="20">
         <v>301</v>
       </c>
@@ -20367,7 +20375,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366" s="20">
         <v>306</v>
       </c>
@@ -20401,7 +20409,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A367" s="20">
         <v>317</v>
       </c>
@@ -20435,7 +20443,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A368" s="20">
         <v>352</v>
       </c>
@@ -20469,7 +20477,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A369" s="20">
         <v>353</v>
       </c>
@@ -20503,7 +20511,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A370" s="20">
         <v>354</v>
       </c>
@@ -20537,7 +20545,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A371" s="20">
         <v>355</v>
       </c>
@@ -20571,7 +20579,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A372" s="20">
         <v>356</v>
       </c>
@@ -20605,7 +20613,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A373" s="20">
         <v>357</v>
       </c>
@@ -20639,7 +20647,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:20" ht="249.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A374" s="20">
         <v>358</v>
       </c>
@@ -20673,7 +20681,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="375" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A375" s="20">
         <v>359</v>
       </c>
@@ -20707,7 +20715,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="376" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A376" s="20">
         <v>360</v>
       </c>
@@ -20741,7 +20749,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="377" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A377" s="20">
         <v>361</v>
       </c>
@@ -20775,7 +20783,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="378" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A378" s="20">
         <v>362</v>
       </c>
@@ -20809,7 +20817,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="379" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A379" s="20">
         <v>363</v>
       </c>
@@ -20843,7 +20851,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="380" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="20">
         <v>364</v>
       </c>
@@ -20877,7 +20885,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A381" s="20">
         <v>365</v>
       </c>
@@ -20911,7 +20919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="382" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A382" s="20">
         <v>366</v>
       </c>

</xml_diff>